<commit_message>
Finished complex scenario for lesson 4
</commit_message>
<xml_diff>
--- a/AndyTEST/src/lesson4/lib/ComplexScenariosChecklist.xlsx
+++ b/AndyTEST/src/lesson4/lib/ComplexScenariosChecklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="285">
   <si>
     <t>Airport-Flight</t>
   </si>
@@ -27,231 +27,12 @@
     <t>Result</t>
   </si>
   <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1001.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1002.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1003.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1004.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1005.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1006.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1007.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1008.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1009.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1010.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1011.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1012.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1013.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1014.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1015.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1016.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1017.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1018.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1019.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1020.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1021.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1022.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1023.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1024.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1025.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1026.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1027.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1028.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1029.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1030.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1031.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1032.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1033.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1034.</t>
-  </si>
-  <si>
-    <t>Check the Duty Free shops of departure airport of flight  #1035.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1001.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1002.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1003.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1004.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1005.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1006.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1007.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1008.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1009.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1010.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1011.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1012.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1013.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1014.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1015.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1016.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1017.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1018.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1019.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1020.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1021.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1022.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1023.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1024.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1025.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1026.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1027.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1028.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1029.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1030.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1031.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1032.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1033.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1034.</t>
-  </si>
-  <si>
-    <t>Check the boarding priority service of departure airport of flight  #1035.</t>
-  </si>
-  <si>
     <t>Flight-Airline</t>
   </si>
   <si>
     <t>Airport-Airline</t>
   </si>
   <si>
-    <t>Check stops number for WizzAir airline of flight #1001.</t>
-  </si>
-  <si>
-    <t>Check average ticket price for WizzAir airline of flight #1001.</t>
-  </si>
-  <si>
-    <t>Check available seats for WizzAir airline of flight #1001.</t>
-  </si>
-  <si>
     <t>Check boarding preority and web regisration for daperture airport of flight #1001</t>
   </si>
   <si>
@@ -460,6 +241,636 @@
   </si>
   <si>
     <t>Check departure airport and airline of flight #1035</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1001</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1002</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1003</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1004</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1005</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1006</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1007</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1008</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1009</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1010</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1011</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1012</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1013</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1014</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1015</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1016</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1017</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1018</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1019</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1020</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1021</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1022</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1023</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1024</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1025</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1026</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1027</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1028</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1029</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1030</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1031</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1032</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1033</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1034</t>
+  </si>
+  <si>
+    <t>Check arrival airport and airline of flight #1035</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1001</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1002</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1003</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1004</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1005</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1006</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1007</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1008</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1009</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1010</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1011</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1012</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1013</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1014</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1015</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1016</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1017</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1018</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1019</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1020</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1021</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1022</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1023</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1024</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1025</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1026</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1027</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1028</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1029</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1030</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1031</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1032</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1033</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1034</t>
+  </si>
+  <si>
+    <t>Check stops number and additional space service of flight #1035</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1001</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1002</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1003</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1004</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1005</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1006</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1007</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1008</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1009</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1010</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1011</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1012</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1013</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1014</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1015</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1016</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1017</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1018</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1019</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1020</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1021</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1022</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1023</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1024</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1025</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1026</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1027</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1028</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1029</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1030</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1031</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1032</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1033</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1034</t>
+  </si>
+  <si>
+    <t>Check average ticket price and Web regisration service of flight #1035</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1001</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1002</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1003</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1004</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1005</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1006</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1007</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1008</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1009</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1010</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1011</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1012</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1013</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1014</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1015</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1016</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1017</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1018</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1019</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1020</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1021</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1022</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1023</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1024</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1025</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1026</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1027</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1028</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1029</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1030</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1031</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1032</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1033</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1034</t>
+  </si>
+  <si>
+    <t>Check available seats and Food service og flight #1035</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1001</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1002</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1003</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1004</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1005</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1006</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1007</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1008</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1009</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1010</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1011</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1012</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1013</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1014</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1015</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1016</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1017</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1018</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1019</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1020</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1021</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1022</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1023</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1024</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1025</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1026</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1027</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1028</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1029</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1030</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1031</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1032</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1033</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1034</t>
+  </si>
+  <si>
+    <t>Check the Duty Free shops and departure airport of flight  #1035</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1001</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1002</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1003</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1004</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1005</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1006</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1007</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1008</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1009</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1010</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1011</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1012</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1013</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1014</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1015</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1016</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1017</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1018</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1019</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1020</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1021</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1022</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1023</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1024</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1025</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1026</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1027</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1028</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1029</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1030</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1031</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1032</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1033</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1034</t>
+  </si>
+  <si>
+    <t>Check the boarding priority service and departure airport of flight  #1035</t>
   </si>
 </sst>
 </file>
@@ -534,7 +945,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -561,6 +972,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -866,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,7 +1312,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -907,7 +1321,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>4</v>
+        <v>216</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -916,7 +1330,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>5</v>
+        <v>217</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -925,7 +1339,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>6</v>
+        <v>218</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -933,8 +1347,8 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>7</v>
+      <c r="B7" s="6" t="s">
+        <v>219</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -943,7 +1357,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>8</v>
+        <v>220</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -952,7 +1366,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>9</v>
+        <v>221</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -961,7 +1375,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>10</v>
+        <v>222</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -970,7 +1384,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>11</v>
+        <v>223</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -979,7 +1393,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>12</v>
+        <v>224</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -988,7 +1402,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>13</v>
+        <v>225</v>
       </c>
       <c r="C13" s="2"/>
     </row>
@@ -997,7 +1411,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>14</v>
+        <v>226</v>
       </c>
       <c r="C14" s="2"/>
     </row>
@@ -1006,7 +1420,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>15</v>
+        <v>227</v>
       </c>
       <c r="C15" s="2"/>
     </row>
@@ -1015,7 +1429,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>16</v>
+        <v>228</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -1024,7 +1438,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>17</v>
+        <v>229</v>
       </c>
       <c r="C17" s="2"/>
     </row>
@@ -1033,7 +1447,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>18</v>
+        <v>230</v>
       </c>
       <c r="C18" s="2"/>
     </row>
@@ -1042,7 +1456,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>19</v>
+        <v>231</v>
       </c>
       <c r="C19" s="2"/>
     </row>
@@ -1051,7 +1465,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>20</v>
+        <v>232</v>
       </c>
       <c r="C20" s="2"/>
     </row>
@@ -1060,7 +1474,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>21</v>
+        <v>233</v>
       </c>
       <c r="C21" s="2"/>
     </row>
@@ -1069,7 +1483,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>22</v>
+        <v>234</v>
       </c>
       <c r="C22" s="2"/>
     </row>
@@ -1078,7 +1492,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="C23" s="2"/>
     </row>
@@ -1087,7 +1501,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>24</v>
+        <v>236</v>
       </c>
       <c r="C24" s="2"/>
     </row>
@@ -1096,7 +1510,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>25</v>
+        <v>237</v>
       </c>
       <c r="C25" s="2"/>
     </row>
@@ -1105,7 +1519,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>26</v>
+        <v>238</v>
       </c>
       <c r="C26" s="2"/>
     </row>
@@ -1114,7 +1528,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>27</v>
+        <v>239</v>
       </c>
       <c r="C27" s="2"/>
     </row>
@@ -1123,7 +1537,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>28</v>
+        <v>240</v>
       </c>
       <c r="C28" s="2"/>
     </row>
@@ -1132,7 +1546,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>29</v>
+        <v>241</v>
       </c>
       <c r="C29" s="2"/>
     </row>
@@ -1141,7 +1555,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>30</v>
+        <v>242</v>
       </c>
       <c r="C30" s="2"/>
     </row>
@@ -1150,7 +1564,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>31</v>
+        <v>243</v>
       </c>
       <c r="C31" s="2"/>
     </row>
@@ -1159,7 +1573,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>32</v>
+        <v>244</v>
       </c>
       <c r="C32" s="2"/>
     </row>
@@ -1168,7 +1582,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>33</v>
+        <v>245</v>
       </c>
       <c r="C33" s="2"/>
     </row>
@@ -1177,7 +1591,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>34</v>
+        <v>246</v>
       </c>
       <c r="C34" s="2"/>
     </row>
@@ -1186,7 +1600,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>35</v>
+        <v>247</v>
       </c>
       <c r="C35" s="2"/>
     </row>
@@ -1195,7 +1609,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>36</v>
+        <v>248</v>
       </c>
       <c r="C36" s="2"/>
     </row>
@@ -1204,7 +1618,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>37</v>
+        <v>249</v>
       </c>
       <c r="C37" s="2"/>
     </row>
@@ -1213,7 +1627,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>38</v>
+        <v>250</v>
       </c>
       <c r="C38" s="2"/>
     </row>
@@ -1222,7 +1636,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>39</v>
+        <v>251</v>
       </c>
       <c r="C39" s="2"/>
     </row>
@@ -1231,7 +1645,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>40</v>
+        <v>252</v>
       </c>
       <c r="C40" s="2"/>
     </row>
@@ -1240,7 +1654,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>41</v>
+        <v>253</v>
       </c>
       <c r="C41" s="2"/>
     </row>
@@ -1249,7 +1663,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>42</v>
+        <v>254</v>
       </c>
       <c r="C42" s="2"/>
     </row>
@@ -1258,7 +1672,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>43</v>
+        <v>255</v>
       </c>
       <c r="C43" s="2"/>
     </row>
@@ -1267,7 +1681,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>44</v>
+        <v>256</v>
       </c>
       <c r="C44" s="2"/>
     </row>
@@ -1276,7 +1690,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>45</v>
+        <v>257</v>
       </c>
       <c r="C45" s="2"/>
     </row>
@@ -1285,7 +1699,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>46</v>
+        <v>258</v>
       </c>
       <c r="C46" s="2"/>
     </row>
@@ -1294,7 +1708,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>47</v>
+        <v>259</v>
       </c>
       <c r="C47" s="2"/>
     </row>
@@ -1303,7 +1717,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>48</v>
+        <v>260</v>
       </c>
       <c r="C48" s="2"/>
     </row>
@@ -1312,7 +1726,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>49</v>
+        <v>261</v>
       </c>
       <c r="C49" s="2"/>
     </row>
@@ -1321,7 +1735,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>50</v>
+        <v>262</v>
       </c>
       <c r="C50" s="2"/>
     </row>
@@ -1330,7 +1744,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>51</v>
+        <v>263</v>
       </c>
       <c r="C51" s="2"/>
     </row>
@@ -1339,7 +1753,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>52</v>
+        <v>264</v>
       </c>
       <c r="C52" s="2"/>
     </row>
@@ -1348,7 +1762,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>53</v>
+        <v>265</v>
       </c>
       <c r="C53" s="2"/>
     </row>
@@ -1357,7 +1771,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>54</v>
+        <v>266</v>
       </c>
       <c r="C54" s="2"/>
     </row>
@@ -1366,7 +1780,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>55</v>
+        <v>267</v>
       </c>
       <c r="C55" s="2"/>
     </row>
@@ -1375,7 +1789,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>56</v>
+        <v>268</v>
       </c>
       <c r="C56" s="2"/>
     </row>
@@ -1384,7 +1798,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>57</v>
+        <v>269</v>
       </c>
       <c r="C57" s="2"/>
     </row>
@@ -1393,7 +1807,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>58</v>
+        <v>270</v>
       </c>
       <c r="C58" s="2"/>
     </row>
@@ -1402,7 +1816,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>59</v>
+        <v>271</v>
       </c>
       <c r="C59" s="2"/>
     </row>
@@ -1411,7 +1825,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>60</v>
+        <v>272</v>
       </c>
       <c r="C60" s="2"/>
     </row>
@@ -1420,7 +1834,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>61</v>
+        <v>273</v>
       </c>
       <c r="C61" s="2"/>
     </row>
@@ -1429,7 +1843,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>62</v>
+        <v>274</v>
       </c>
       <c r="C62" s="2"/>
     </row>
@@ -1438,7 +1852,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>63</v>
+        <v>275</v>
       </c>
       <c r="C63" s="2"/>
     </row>
@@ -1447,7 +1861,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>64</v>
+        <v>276</v>
       </c>
       <c r="C64" s="2"/>
     </row>
@@ -1456,7 +1870,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>65</v>
+        <v>277</v>
       </c>
       <c r="C65" s="2"/>
     </row>
@@ -1465,7 +1879,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>66</v>
+        <v>278</v>
       </c>
       <c r="C66" s="2"/>
     </row>
@@ -1474,7 +1888,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>67</v>
+        <v>279</v>
       </c>
       <c r="C67" s="2"/>
     </row>
@@ -1483,7 +1897,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>68</v>
+        <v>280</v>
       </c>
       <c r="C68" s="2"/>
     </row>
@@ -1492,7 +1906,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>69</v>
+        <v>281</v>
       </c>
       <c r="C69" s="2"/>
     </row>
@@ -1501,7 +1915,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>70</v>
+        <v>282</v>
       </c>
       <c r="C70" s="2"/>
     </row>
@@ -1510,7 +1924,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>71</v>
+        <v>283</v>
       </c>
       <c r="C71" s="2"/>
     </row>
@@ -1519,7 +1933,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>72</v>
+        <v>284</v>
       </c>
       <c r="C72" s="2"/>
     </row>
@@ -1531,20 +1945,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C177"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E159" sqref="E159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="49.75" customWidth="1"/>
+    <col min="2" max="2" width="55.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="8"/>
@@ -1563,7 +1977,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>113</v>
+        <v>40</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -1572,7 +1986,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -1581,7 +1995,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>115</v>
+        <v>42</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -1590,7 +2004,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>116</v>
+        <v>43</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -1599,7 +2013,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>117</v>
+        <v>44</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -1608,7 +2022,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -1617,7 +2031,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>119</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -1626,7 +2040,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>120</v>
+        <v>47</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -1635,7 +2049,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>121</v>
+        <v>48</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -1644,7 +2058,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>122</v>
+        <v>49</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -1653,7 +2067,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>123</v>
+        <v>50</v>
       </c>
       <c r="C13" s="2"/>
     </row>
@@ -1662,7 +2076,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>124</v>
+        <v>51</v>
       </c>
       <c r="C14" s="2"/>
     </row>
@@ -1671,7 +2085,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>125</v>
+        <v>52</v>
       </c>
       <c r="C15" s="2"/>
     </row>
@@ -1680,7 +2094,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>126</v>
+        <v>53</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -1689,7 +2103,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>127</v>
+        <v>54</v>
       </c>
       <c r="C17" s="2"/>
     </row>
@@ -1698,7 +2112,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="C18" s="2"/>
     </row>
@@ -1707,7 +2121,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>129</v>
+        <v>56</v>
       </c>
       <c r="C19" s="2"/>
     </row>
@@ -1716,7 +2130,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>130</v>
+        <v>57</v>
       </c>
       <c r="C20" s="2"/>
     </row>
@@ -1725,7 +2139,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>131</v>
+        <v>58</v>
       </c>
       <c r="C21" s="2"/>
     </row>
@@ -1734,7 +2148,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>132</v>
+        <v>59</v>
       </c>
       <c r="C22" s="2"/>
     </row>
@@ -1743,7 +2157,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>133</v>
+        <v>60</v>
       </c>
       <c r="C23" s="2"/>
     </row>
@@ -1752,7 +2166,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>134</v>
+        <v>61</v>
       </c>
       <c r="C24" s="2"/>
     </row>
@@ -1761,7 +2175,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>135</v>
+        <v>62</v>
       </c>
       <c r="C25" s="2"/>
     </row>
@@ -1770,7 +2184,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C26" s="2"/>
     </row>
@@ -1779,7 +2193,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>137</v>
+        <v>64</v>
       </c>
       <c r="C27" s="2"/>
     </row>
@@ -1788,7 +2202,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>138</v>
+        <v>65</v>
       </c>
       <c r="C28" s="2"/>
     </row>
@@ -1797,7 +2211,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>139</v>
+        <v>66</v>
       </c>
       <c r="C29" s="2"/>
     </row>
@@ -1806,7 +2220,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>140</v>
+        <v>67</v>
       </c>
       <c r="C30" s="2"/>
     </row>
@@ -1815,7 +2229,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>141</v>
+        <v>68</v>
       </c>
       <c r="C31" s="2"/>
     </row>
@@ -1824,7 +2238,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="C32" s="2"/>
     </row>
@@ -1833,7 +2247,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>143</v>
+        <v>70</v>
       </c>
       <c r="C33" s="2"/>
     </row>
@@ -1842,7 +2256,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>144</v>
+        <v>71</v>
       </c>
       <c r="C34" s="2"/>
     </row>
@@ -1851,7 +2265,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>145</v>
+        <v>72</v>
       </c>
       <c r="C35" s="2"/>
     </row>
@@ -1860,7 +2274,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>146</v>
+        <v>73</v>
       </c>
       <c r="C36" s="2"/>
     </row>
@@ -1869,24 +2283,1269 @@
         <v>35</v>
       </c>
       <c r="B37" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>36</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>37</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>38</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>39</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>40</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="2"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>41</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="2"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>42</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" s="2"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>43</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>44</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>45</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" s="2"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>46</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>47</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>48</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C50" s="2"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>49</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" s="2"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>50</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" s="2"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>51</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="2"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>52</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>53</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C55" s="2"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>54</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C56" s="2"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>55</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" s="2"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>56</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C58" s="2"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>57</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59" s="2"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>58</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60" s="2"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>59</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C61" s="2"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>60</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>61</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>62</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C64" s="2"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>63</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C65" s="2"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>64</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C66" s="2"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>65</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C67" s="2"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>66</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C68" s="2"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>67</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C69" s="2"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>68</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C70" s="2"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>69</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C71" s="2"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>70</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C72" s="2"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>71</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C73" s="2"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>72</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C74" s="2"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>73</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C75" s="2"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>74</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C76" s="2"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>75</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C77" s="2"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>76</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C78" s="2"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>77</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C79" s="2"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>78</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C80" s="2"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>79</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C81" s="2"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>80</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C82" s="2"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>81</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C83" s="2"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>82</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C84" s="2"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>83</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C85" s="2"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>84</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C86" s="2"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>85</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C87" s="2"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>86</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C88" s="2"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>87</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C89" s="2"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>88</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C90" s="2"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>89</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C91" s="2"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>90</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C92" s="2"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>91</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C93" s="2"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>92</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C94" s="2"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>93</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C95" s="2"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>94</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C96" s="2"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>95</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C97" s="2"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>96</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C98" s="2"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>97</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C99" s="2"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>98</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C100" s="2"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>99</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C101" s="2"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>100</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C102" s="2"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>101</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C103" s="2"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="2">
+        <v>102</v>
+      </c>
+      <c r="B104" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C104" s="2"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="2">
+        <v>103</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C105" s="2"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="2">
+        <v>104</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C106" s="2"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
+        <v>105</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C107" s="2"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
+        <v>106</v>
+      </c>
+      <c r="B108" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C108" s="2"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="2">
+        <v>107</v>
+      </c>
+      <c r="B109" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C109" s="2"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
+        <v>108</v>
+      </c>
+      <c r="B110" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="C37" s="2"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="6" t="s">
-        <v>77</v>
-      </c>
+      <c r="C110" s="2"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
+        <v>109</v>
+      </c>
+      <c r="B111" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C111" s="2"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
+        <v>110</v>
+      </c>
+      <c r="B112" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C112" s="2"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="2">
+        <v>111</v>
+      </c>
+      <c r="B113" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C113" s="2"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="2">
+        <v>112</v>
+      </c>
+      <c r="B114" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C114" s="2"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="2">
+        <v>113</v>
+      </c>
+      <c r="B115" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C115" s="2"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="2">
+        <v>114</v>
+      </c>
+      <c r="B116" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C116" s="2"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="2">
+        <v>115</v>
+      </c>
+      <c r="B117" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C117" s="2"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="2">
+        <v>116</v>
+      </c>
+      <c r="B118" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C118" s="2"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="2">
+        <v>117</v>
+      </c>
+      <c r="B119" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C119" s="2"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="2">
+        <v>118</v>
+      </c>
+      <c r="B120" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C120" s="2"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="2">
+        <v>119</v>
+      </c>
+      <c r="B121" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C121" s="2"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="2">
+        <v>120</v>
+      </c>
+      <c r="B122" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C122" s="2"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="2">
+        <v>121</v>
+      </c>
+      <c r="B123" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C123" s="2"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="2">
+        <v>122</v>
+      </c>
+      <c r="B124" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C124" s="2"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="2">
+        <v>123</v>
+      </c>
+      <c r="B125" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C125" s="2"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="2">
+        <v>124</v>
+      </c>
+      <c r="B126" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C126" s="2"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="2">
+        <v>125</v>
+      </c>
+      <c r="B127" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="C127" s="2"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="2">
+        <v>126</v>
+      </c>
+      <c r="B128" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="C128" s="2"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="2">
+        <v>127</v>
+      </c>
+      <c r="B129" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C129" s="2"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="2">
+        <v>128</v>
+      </c>
+      <c r="B130" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C130" s="2"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="2">
+        <v>129</v>
+      </c>
+      <c r="B131" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C131" s="2"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="2">
+        <v>130</v>
+      </c>
+      <c r="B132" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C132" s="2"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="2">
+        <v>131</v>
+      </c>
+      <c r="B133" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C133" s="2"/>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="2">
+        <v>132</v>
+      </c>
+      <c r="B134" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C134" s="2"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="2">
+        <v>133</v>
+      </c>
+      <c r="B135" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="C135" s="2"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="2">
+        <v>134</v>
+      </c>
+      <c r="B136" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C136" s="2"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="2">
+        <v>135</v>
+      </c>
+      <c r="B137" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C137" s="2"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="2">
+        <v>136</v>
+      </c>
+      <c r="B138" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C138" s="2"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="2">
+        <v>137</v>
+      </c>
+      <c r="B139" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="C139" s="2"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="2">
+        <v>138</v>
+      </c>
+      <c r="B140" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="C140" s="2"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="2">
+        <v>139</v>
+      </c>
+      <c r="B141" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C141" s="2"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="2">
+        <v>140</v>
+      </c>
+      <c r="B142" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C142" s="2"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="2">
+        <v>141</v>
+      </c>
+      <c r="B143" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C143" s="2"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="2">
+        <v>142</v>
+      </c>
+      <c r="B144" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C144" s="2"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="2">
+        <v>143</v>
+      </c>
+      <c r="B145" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C145" s="2"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="2">
+        <v>144</v>
+      </c>
+      <c r="B146" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C146" s="2"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="2">
+        <v>145</v>
+      </c>
+      <c r="B147" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="C147" s="2"/>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="2">
+        <v>146</v>
+      </c>
+      <c r="B148" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C148" s="2"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="2">
+        <v>147</v>
+      </c>
+      <c r="B149" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="C149" s="2"/>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="2">
+        <v>148</v>
+      </c>
+      <c r="B150" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="C150" s="2"/>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="2">
+        <v>149</v>
+      </c>
+      <c r="B151" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C151" s="2"/>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="2">
+        <v>150</v>
+      </c>
+      <c r="B152" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C152" s="2"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="2">
+        <v>151</v>
+      </c>
+      <c r="B153" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C153" s="2"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="2">
+        <v>152</v>
+      </c>
+      <c r="B154" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="C154" s="2"/>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="2">
+        <v>153</v>
+      </c>
+      <c r="B155" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C155" s="2"/>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="2">
+        <v>154</v>
+      </c>
+      <c r="B156" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C156" s="2"/>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="2">
+        <v>155</v>
+      </c>
+      <c r="B157" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C157" s="2"/>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="2">
+        <v>156</v>
+      </c>
+      <c r="B158" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="C158" s="2"/>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="2">
+        <v>157</v>
+      </c>
+      <c r="B159" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C159" s="2"/>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="2">
+        <v>158</v>
+      </c>
+      <c r="B160" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C160" s="2"/>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="2">
+        <v>159</v>
+      </c>
+      <c r="B161" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="C161" s="2"/>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="2">
+        <v>160</v>
+      </c>
+      <c r="B162" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C162" s="2"/>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="2">
+        <v>161</v>
+      </c>
+      <c r="B163" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C163" s="2"/>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="2">
+        <v>162</v>
+      </c>
+      <c r="B164" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C164" s="2"/>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="2">
+        <v>163</v>
+      </c>
+      <c r="B165" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C165" s="2"/>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="2">
+        <v>164</v>
+      </c>
+      <c r="B166" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C166" s="2"/>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="2">
+        <v>165</v>
+      </c>
+      <c r="B167" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="C167" s="2"/>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="2">
+        <v>166</v>
+      </c>
+      <c r="B168" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C168" s="2"/>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="2">
+        <v>167</v>
+      </c>
+      <c r="B169" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C169" s="2"/>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="2">
+        <v>168</v>
+      </c>
+      <c r="B170" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C170" s="2"/>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="2">
+        <v>169</v>
+      </c>
+      <c r="B171" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C171" s="2"/>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="2">
+        <v>170</v>
+      </c>
+      <c r="B172" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C172" s="2"/>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="2">
+        <v>171</v>
+      </c>
+      <c r="B173" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C173" s="2"/>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="2">
+        <v>172</v>
+      </c>
+      <c r="B174" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C174" s="2"/>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="2">
+        <v>173</v>
+      </c>
+      <c r="B175" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C175" s="2"/>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="2">
+        <v>174</v>
+      </c>
+      <c r="B176" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C176" s="2"/>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="2">
+        <v>175</v>
+      </c>
+      <c r="B177" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C177" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1908,7 +3567,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>74</v>
+        <v>4</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="8"/>
@@ -1927,7 +3586,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -1936,7 +3595,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>79</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -1945,7 +3604,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -1954,7 +3613,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>81</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -1963,7 +3622,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -1972,7 +3631,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -1981,7 +3640,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -1990,7 +3649,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>85</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -1999,7 +3658,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -2008,7 +3667,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -2017,7 +3676,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>88</v>
+        <v>15</v>
       </c>
       <c r="C13" s="2"/>
     </row>
@@ -2026,7 +3685,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="C14" s="2"/>
     </row>
@@ -2035,7 +3694,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>90</v>
+        <v>17</v>
       </c>
       <c r="C15" s="2"/>
     </row>
@@ -2044,7 +3703,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>91</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -2053,7 +3712,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>92</v>
+        <v>19</v>
       </c>
       <c r="C17" s="2"/>
     </row>
@@ -2062,7 +3721,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="C18" s="2"/>
     </row>
@@ -2071,7 +3730,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="C19" s="2"/>
     </row>
@@ -2080,7 +3739,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="C20" s="2"/>
     </row>
@@ -2089,7 +3748,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="C21" s="2"/>
     </row>
@@ -2098,7 +3757,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="C22" s="2"/>
     </row>
@@ -2107,7 +3766,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>98</v>
+        <v>25</v>
       </c>
       <c r="C23" s="2"/>
     </row>
@@ -2116,7 +3775,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="C24" s="2"/>
     </row>
@@ -2125,7 +3784,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="C25" s="2"/>
     </row>
@@ -2134,7 +3793,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="C26" s="2"/>
     </row>
@@ -2143,7 +3802,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="C27" s="2"/>
     </row>
@@ -2152,7 +3811,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>103</v>
+        <v>30</v>
       </c>
       <c r="C28" s="2"/>
     </row>
@@ -2161,7 +3820,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>104</v>
+        <v>31</v>
       </c>
       <c r="C29" s="2"/>
     </row>
@@ -2170,7 +3829,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="C30" s="2"/>
     </row>
@@ -2179,7 +3838,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="C31" s="2"/>
     </row>
@@ -2188,7 +3847,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>107</v>
+        <v>34</v>
       </c>
       <c r="C32" s="2"/>
     </row>
@@ -2197,7 +3856,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>108</v>
+        <v>35</v>
       </c>
       <c r="C33" s="2"/>
     </row>
@@ -2206,7 +3865,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>109</v>
+        <v>36</v>
       </c>
       <c r="C34" s="2"/>
     </row>
@@ -2215,7 +3874,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>110</v>
+        <v>37</v>
       </c>
       <c r="C35" s="2"/>
     </row>
@@ -2224,7 +3883,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
       <c r="C36" s="2"/>
     </row>
@@ -2233,7 +3892,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>112</v>
+        <v>39</v>
       </c>
       <c r="C37" s="2"/>
     </row>

</xml_diff>